<commit_message>
added the relevant constructs to be checked in data presence file
</commit_message>
<xml_diff>
--- a/docs/20240121-variables.xlsx
+++ b/docs/20240121-variables.xlsx
@@ -8,17 +8,28 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://solisservices.sharepoint.com/sites/ICITOP/Shared Documents/General/data renaming/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0650324F-0FD8-43DD-8BCD-5D3475258605}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="8_{0650324F-0FD8-43DD-8BCD-5D3475258605}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5AB3106E-0D92-4A06-B96C-9FD3174A9C86}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -763,9 +774,6 @@
     <t>G2 substance use</t>
   </si>
   <si>
-    <t>bob</t>
-  </si>
-  <si>
     <t>example</t>
   </si>
   <si>
@@ -784,9 +792,6 @@
     <t>g1w[1,2,3, etc][reporter][target][type]par</t>
   </si>
   <si>
-    <t>g1w[1,2,etc][reporter][target][type]vinc</t>
-  </si>
-  <si>
     <t>g1w[1,2,etc][reporter][target][type]occ</t>
   </si>
   <si>
@@ -850,9 +855,6 @@
     <t>g2[v1,2 etc/w1,2 etc][reporter][target][type]gen</t>
   </si>
   <si>
-    <t>g2[v1,2 etc/w1,2 etc][reporter][target][type]bob</t>
-  </si>
-  <si>
     <t>g2[v1,2 etc/w1,2 etc][reporter][target][type]cst</t>
   </si>
   <si>
@@ -914,6 +916,15 @@
   </si>
   <si>
     <t>g3[v1,2 etc/w1,2 etc][reporter][target][type]bir</t>
+  </si>
+  <si>
+    <t>inc</t>
+  </si>
+  <si>
+    <t>g1w[1,2,etc][reporter][target][type]inc</t>
+  </si>
+  <si>
+    <t>g2[v1,2 etc/w1,2 etc][reporter][target][type]bir</t>
   </si>
 </sst>
 </file>
@@ -1462,8 +1473,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AM70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D55" sqref="D55:D67"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1499,7 +1510,7 @@
   <sheetData>
     <row r="1" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A1" s="15" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B1" s="15" t="s">
         <v>58</v>
@@ -1724,10 +1735,10 @@
     </row>
     <row r="4" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="12" spans="1:39" s="4" customFormat="1" x14ac:dyDescent="0.35">
@@ -1750,10 +1761,10 @@
     </row>
     <row r="13" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D13" s="19"/>
       <c r="E13" s="20"/>
@@ -1987,7 +1998,7 @@
         <v>42</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D19" s="10" t="s">
         <v>41</v>
@@ -2100,13 +2111,13 @@
     </row>
     <row r="20" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>59</v>
+        <v>136</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>15</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>95</v>
+        <v>137</v>
       </c>
     </row>
     <row r="21" spans="1:39" x14ac:dyDescent="0.35">
@@ -2117,7 +2128,7 @@
         <v>14</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="22" spans="1:39" x14ac:dyDescent="0.35">
@@ -2128,29 +2139,29 @@
         <v>13</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="23" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="24" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B24" s="17" t="s">
         <v>85</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="25" spans="1:39" x14ac:dyDescent="0.35">
@@ -2161,7 +2172,7 @@
         <v>38</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="26" spans="1:39" x14ac:dyDescent="0.35">
@@ -2172,7 +2183,7 @@
         <v>37</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="27" spans="1:39" x14ac:dyDescent="0.35">
@@ -2183,7 +2194,7 @@
         <v>36</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="28" spans="1:39" x14ac:dyDescent="0.35">
@@ -2194,7 +2205,7 @@
         <v>35</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="29" spans="1:39" x14ac:dyDescent="0.35">
@@ -2205,18 +2216,18 @@
         <v>34</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="30" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="31" spans="1:39" x14ac:dyDescent="0.35">
@@ -2227,7 +2238,7 @@
         <v>32</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="32" spans="1:39" x14ac:dyDescent="0.35">
@@ -2238,7 +2249,7 @@
         <v>31</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="33" spans="1:39" x14ac:dyDescent="0.35">
@@ -2249,18 +2260,18 @@
         <v>30</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="34" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>29</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="36" spans="1:39" s="4" customFormat="1" x14ac:dyDescent="0.35">
@@ -2289,7 +2300,7 @@
         <v>27</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="38" spans="1:39" x14ac:dyDescent="0.35">
@@ -2300,7 +2311,7 @@
         <v>26</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="39" spans="1:39" x14ac:dyDescent="0.35">
@@ -2311,7 +2322,7 @@
         <v>25</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="40" spans="1:39" x14ac:dyDescent="0.35">
@@ -2322,18 +2333,18 @@
         <v>24</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="41" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>23</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>117</v>
+        <v>138</v>
       </c>
     </row>
     <row r="42" spans="1:39" x14ac:dyDescent="0.35">
@@ -2344,18 +2355,18 @@
         <v>21</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="43" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A43" s="18" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B43" s="17" t="s">
         <v>7</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="44" spans="1:39" x14ac:dyDescent="0.35">
@@ -2389,7 +2400,7 @@
         <v>9</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="47" spans="1:39" x14ac:dyDescent="0.35">
@@ -2400,7 +2411,7 @@
         <v>20</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="48" spans="1:39" x14ac:dyDescent="0.35">
@@ -2411,7 +2422,7 @@
         <v>19</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="49" spans="1:39" x14ac:dyDescent="0.35">
@@ -2422,7 +2433,7 @@
         <v>18</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="50" spans="1:39" x14ac:dyDescent="0.35">
@@ -2433,7 +2444,7 @@
         <v>17</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="51" spans="1:39" x14ac:dyDescent="0.35">
@@ -2444,7 +2455,7 @@
         <v>16</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="52" spans="1:39" x14ac:dyDescent="0.35">
@@ -2455,7 +2466,7 @@
         <v>15</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="53" spans="1:39" x14ac:dyDescent="0.35">
@@ -2466,7 +2477,7 @@
         <v>14</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="54" spans="1:39" x14ac:dyDescent="0.35">
@@ -2477,18 +2488,18 @@
         <v>13</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="55" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B55" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="56" spans="1:39" x14ac:dyDescent="0.35">
@@ -2499,7 +2510,7 @@
         <v>11</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="57" spans="1:39" x14ac:dyDescent="0.35">
@@ -2510,7 +2521,7 @@
         <v>10</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="58" spans="1:39" x14ac:dyDescent="0.35">
@@ -2521,7 +2532,7 @@
         <v>9</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="59" spans="1:39" x14ac:dyDescent="0.35">
@@ -2532,7 +2543,7 @@
         <v>8</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="60" spans="1:39" x14ac:dyDescent="0.35">
@@ -2543,7 +2554,7 @@
         <v>87</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="61" spans="1:39" s="4" customFormat="1" x14ac:dyDescent="0.35">
@@ -2572,7 +2583,7 @@
         <v>5</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="63" spans="1:39" x14ac:dyDescent="0.35">
@@ -2583,7 +2594,7 @@
         <v>4</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="64" spans="1:39" x14ac:dyDescent="0.35">
@@ -2594,7 +2605,7 @@
         <v>3</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="65" spans="1:39" x14ac:dyDescent="0.35">
@@ -2605,7 +2616,7 @@
         <v>2</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="66" spans="1:39" x14ac:dyDescent="0.35">
@@ -2616,7 +2627,7 @@
         <v>1</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="68" spans="1:39" s="4" customFormat="1" x14ac:dyDescent="0.35">
@@ -2672,12 +2683,14 @@
     <mergeCell ref="V17:X17"/>
     <mergeCell ref="Y17:AA17"/>
     <mergeCell ref="S17:U17"/>
+    <mergeCell ref="P17:R17"/>
     <mergeCell ref="V16:X16"/>
     <mergeCell ref="Y16:AA16"/>
     <mergeCell ref="P16:R16"/>
     <mergeCell ref="Y14:AA14"/>
     <mergeCell ref="AB16:AD16"/>
     <mergeCell ref="S15:U15"/>
+    <mergeCell ref="V14:X14"/>
     <mergeCell ref="J15:L15"/>
     <mergeCell ref="M15:O15"/>
     <mergeCell ref="P15:R15"/>
@@ -2689,7 +2702,11 @@
     <mergeCell ref="G13:I13"/>
     <mergeCell ref="G14:I14"/>
     <mergeCell ref="G15:I15"/>
-    <mergeCell ref="P17:R17"/>
+    <mergeCell ref="J14:L14"/>
+    <mergeCell ref="J1:L1"/>
+    <mergeCell ref="J13:L13"/>
+    <mergeCell ref="M13:O13"/>
+    <mergeCell ref="M1:O1"/>
     <mergeCell ref="D18:F18"/>
     <mergeCell ref="D17:F17"/>
     <mergeCell ref="S16:U16"/>
@@ -2701,12 +2718,6 @@
     <mergeCell ref="M17:O17"/>
     <mergeCell ref="D16:F16"/>
     <mergeCell ref="G16:I16"/>
-    <mergeCell ref="J14:L14"/>
-    <mergeCell ref="V14:X14"/>
-    <mergeCell ref="J1:L1"/>
-    <mergeCell ref="J13:L13"/>
-    <mergeCell ref="M13:O13"/>
-    <mergeCell ref="M1:O1"/>
     <mergeCell ref="P1:R1"/>
     <mergeCell ref="M14:O14"/>
     <mergeCell ref="P14:R14"/>

</xml_diff>

<commit_message>
worked on renaming 44.us-eat + made small changes to docs variables and moderators
</commit_message>
<xml_diff>
--- a/docs/20240121-variables.xlsx
+++ b/docs/20240121-variables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://solisservices.sharepoint.com/sites/ICITOP/Shared Documents/General/data renaming/docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="O:\Research\FSW\Research_data\JG\SanneG\ICITOP IPD_MA\icitop\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="8_{0650324F-0FD8-43DD-8BCD-5D3475258605}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5AB3106E-0D92-4A06-B96C-9FD3174A9C86}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5376A5AB-CD13-4ABD-8E7C-13158F7CD5F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
@@ -870,9 +870,6 @@
     <t>g2[v1,2 etc/w1,2 etc][reporter][target][type]car</t>
   </si>
   <si>
-    <t>g2[v1,2 etc/w1,2 etc][reporter][target][type]etp</t>
-  </si>
-  <si>
     <t>g2[v1,2 etc/w1,2 etc][reporter][target][type]res</t>
   </si>
   <si>
@@ -925,6 +922,9 @@
   </si>
   <si>
     <t>g2[v1,2 etc/w1,2 etc][reporter][target][type]bir</t>
+  </si>
+  <si>
+    <t>g2[v1,2 etc/w1,2 etc][reporter]r etp</t>
   </si>
 </sst>
 </file>
@@ -1139,6 +1139,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1146,15 +1155,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1473,8 +1473,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AM70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1518,66 +1518,66 @@
       <c r="C1" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="D1" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="E1" s="26"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="25" t="s">
+      <c r="E1" s="23"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="H1" s="26"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="25" t="s">
+      <c r="H1" s="23"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="K1" s="26"/>
-      <c r="L1" s="27"/>
-      <c r="M1" s="25" t="s">
+      <c r="K1" s="23"/>
+      <c r="L1" s="24"/>
+      <c r="M1" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="N1" s="26"/>
-      <c r="O1" s="27"/>
-      <c r="P1" s="25" t="s">
+      <c r="N1" s="23"/>
+      <c r="O1" s="24"/>
+      <c r="P1" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="Q1" s="26"/>
-      <c r="R1" s="27"/>
-      <c r="S1" s="25" t="s">
+      <c r="Q1" s="23"/>
+      <c r="R1" s="24"/>
+      <c r="S1" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="T1" s="26"/>
-      <c r="U1" s="27"/>
-      <c r="V1" s="25" t="s">
+      <c r="T1" s="23"/>
+      <c r="U1" s="24"/>
+      <c r="V1" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="W1" s="26"/>
-      <c r="X1" s="27"/>
-      <c r="Y1" s="25" t="s">
+      <c r="W1" s="23"/>
+      <c r="X1" s="24"/>
+      <c r="Y1" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="Z1" s="26"/>
-      <c r="AA1" s="27"/>
-      <c r="AB1" s="22" t="s">
+      <c r="Z1" s="23"/>
+      <c r="AA1" s="24"/>
+      <c r="AB1" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="AC1" s="23"/>
-      <c r="AD1" s="24"/>
-      <c r="AE1" s="22" t="s">
+      <c r="AC1" s="26"/>
+      <c r="AD1" s="27"/>
+      <c r="AE1" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="AF1" s="23"/>
-      <c r="AG1" s="24"/>
-      <c r="AH1" s="22" t="s">
+      <c r="AF1" s="26"/>
+      <c r="AG1" s="27"/>
+      <c r="AH1" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="AI1" s="23"/>
-      <c r="AJ1" s="24"/>
-      <c r="AK1" s="22" t="s">
+      <c r="AI1" s="26"/>
+      <c r="AJ1" s="27"/>
+      <c r="AK1" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="AL1" s="23"/>
-      <c r="AM1" s="24"/>
+      <c r="AL1" s="26"/>
+      <c r="AM1" s="27"/>
     </row>
     <row r="2" spans="1:39" x14ac:dyDescent="0.35">
       <c r="B2" s="11"/>
@@ -2111,13 +2111,13 @@
     </row>
     <row r="20" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>15</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="21" spans="1:39" x14ac:dyDescent="0.35">
@@ -2344,7 +2344,7 @@
         <v>23</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="42" spans="1:39" x14ac:dyDescent="0.35">
@@ -2433,7 +2433,7 @@
         <v>18</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>120</v>
+        <v>138</v>
       </c>
     </row>
     <row r="50" spans="1:39" x14ac:dyDescent="0.35">
@@ -2444,7 +2444,7 @@
         <v>17</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="51" spans="1:39" x14ac:dyDescent="0.35">
@@ -2455,7 +2455,7 @@
         <v>16</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="52" spans="1:39" x14ac:dyDescent="0.35">
@@ -2466,7 +2466,7 @@
         <v>15</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="53" spans="1:39" x14ac:dyDescent="0.35">
@@ -2477,7 +2477,7 @@
         <v>14</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="54" spans="1:39" x14ac:dyDescent="0.35">
@@ -2488,7 +2488,7 @@
         <v>13</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="55" spans="1:39" x14ac:dyDescent="0.35">
@@ -2499,7 +2499,7 @@
         <v>12</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="56" spans="1:39" x14ac:dyDescent="0.35">
@@ -2510,7 +2510,7 @@
         <v>11</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="57" spans="1:39" x14ac:dyDescent="0.35">
@@ -2521,7 +2521,7 @@
         <v>10</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="58" spans="1:39" x14ac:dyDescent="0.35">
@@ -2543,7 +2543,7 @@
         <v>8</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="60" spans="1:39" x14ac:dyDescent="0.35">
@@ -2554,7 +2554,7 @@
         <v>87</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="61" spans="1:39" s="4" customFormat="1" x14ac:dyDescent="0.35">
@@ -2583,7 +2583,7 @@
         <v>5</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="63" spans="1:39" x14ac:dyDescent="0.35">
@@ -2594,7 +2594,7 @@
         <v>4</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="64" spans="1:39" x14ac:dyDescent="0.35">
@@ -2605,7 +2605,7 @@
         <v>3</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="65" spans="1:39" x14ac:dyDescent="0.35">
@@ -2616,7 +2616,7 @@
         <v>2</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="66" spans="1:39" x14ac:dyDescent="0.35">
@@ -2627,7 +2627,7 @@
         <v>1</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="68" spans="1:39" s="4" customFormat="1" x14ac:dyDescent="0.35">
@@ -2672,25 +2672,55 @@
     </row>
   </sheetData>
   <mergeCells count="84">
-    <mergeCell ref="AB17:AD17"/>
-    <mergeCell ref="AB18:AD18"/>
-    <mergeCell ref="J18:L18"/>
-    <mergeCell ref="M18:O18"/>
-    <mergeCell ref="P18:R18"/>
-    <mergeCell ref="S18:U18"/>
-    <mergeCell ref="V18:X18"/>
-    <mergeCell ref="Y18:AA18"/>
-    <mergeCell ref="V17:X17"/>
-    <mergeCell ref="Y17:AA17"/>
-    <mergeCell ref="S17:U17"/>
-    <mergeCell ref="P17:R17"/>
-    <mergeCell ref="V16:X16"/>
-    <mergeCell ref="Y16:AA16"/>
-    <mergeCell ref="P16:R16"/>
-    <mergeCell ref="Y14:AA14"/>
-    <mergeCell ref="AB16:AD16"/>
-    <mergeCell ref="S15:U15"/>
-    <mergeCell ref="V14:X14"/>
+    <mergeCell ref="AH17:AJ17"/>
+    <mergeCell ref="AH18:AJ18"/>
+    <mergeCell ref="AK18:AM18"/>
+    <mergeCell ref="AE16:AG16"/>
+    <mergeCell ref="AH16:AJ16"/>
+    <mergeCell ref="AK16:AM16"/>
+    <mergeCell ref="AK17:AM17"/>
+    <mergeCell ref="AE18:AG18"/>
+    <mergeCell ref="AE17:AG17"/>
+    <mergeCell ref="AK14:AM14"/>
+    <mergeCell ref="V15:X15"/>
+    <mergeCell ref="Y15:AA15"/>
+    <mergeCell ref="AB15:AD15"/>
+    <mergeCell ref="AE15:AG15"/>
+    <mergeCell ref="AH15:AJ15"/>
+    <mergeCell ref="AK15:AM15"/>
+    <mergeCell ref="AB14:AD14"/>
+    <mergeCell ref="AE14:AG14"/>
+    <mergeCell ref="AH14:AJ14"/>
+    <mergeCell ref="AK1:AM1"/>
+    <mergeCell ref="V13:X13"/>
+    <mergeCell ref="Y13:AA13"/>
+    <mergeCell ref="AB13:AD13"/>
+    <mergeCell ref="AE13:AG13"/>
+    <mergeCell ref="AH13:AJ13"/>
+    <mergeCell ref="AK13:AM13"/>
+    <mergeCell ref="V1:X1"/>
+    <mergeCell ref="Y1:AA1"/>
+    <mergeCell ref="AB1:AD1"/>
+    <mergeCell ref="AE1:AG1"/>
+    <mergeCell ref="AH1:AJ1"/>
+    <mergeCell ref="P1:R1"/>
+    <mergeCell ref="M14:O14"/>
+    <mergeCell ref="P14:R14"/>
+    <mergeCell ref="S14:U14"/>
+    <mergeCell ref="S1:U1"/>
+    <mergeCell ref="P13:R13"/>
+    <mergeCell ref="S13:U13"/>
+    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="D17:F17"/>
+    <mergeCell ref="S16:U16"/>
+    <mergeCell ref="G17:I17"/>
+    <mergeCell ref="G18:I18"/>
+    <mergeCell ref="J16:L16"/>
+    <mergeCell ref="M16:O16"/>
+    <mergeCell ref="J17:L17"/>
+    <mergeCell ref="M17:O17"/>
+    <mergeCell ref="D16:F16"/>
+    <mergeCell ref="G16:I16"/>
     <mergeCell ref="J15:L15"/>
     <mergeCell ref="M15:O15"/>
     <mergeCell ref="P15:R15"/>
@@ -2707,55 +2737,25 @@
     <mergeCell ref="J13:L13"/>
     <mergeCell ref="M13:O13"/>
     <mergeCell ref="M1:O1"/>
-    <mergeCell ref="D18:F18"/>
-    <mergeCell ref="D17:F17"/>
-    <mergeCell ref="S16:U16"/>
-    <mergeCell ref="G17:I17"/>
-    <mergeCell ref="G18:I18"/>
-    <mergeCell ref="J16:L16"/>
-    <mergeCell ref="M16:O16"/>
-    <mergeCell ref="J17:L17"/>
-    <mergeCell ref="M17:O17"/>
-    <mergeCell ref="D16:F16"/>
-    <mergeCell ref="G16:I16"/>
-    <mergeCell ref="P1:R1"/>
-    <mergeCell ref="M14:O14"/>
-    <mergeCell ref="P14:R14"/>
-    <mergeCell ref="S14:U14"/>
-    <mergeCell ref="S1:U1"/>
-    <mergeCell ref="P13:R13"/>
-    <mergeCell ref="S13:U13"/>
-    <mergeCell ref="AK1:AM1"/>
-    <mergeCell ref="V13:X13"/>
-    <mergeCell ref="Y13:AA13"/>
-    <mergeCell ref="AB13:AD13"/>
-    <mergeCell ref="AE13:AG13"/>
-    <mergeCell ref="AH13:AJ13"/>
-    <mergeCell ref="AK13:AM13"/>
-    <mergeCell ref="V1:X1"/>
-    <mergeCell ref="Y1:AA1"/>
-    <mergeCell ref="AB1:AD1"/>
-    <mergeCell ref="AE1:AG1"/>
-    <mergeCell ref="AH1:AJ1"/>
-    <mergeCell ref="AK14:AM14"/>
-    <mergeCell ref="V15:X15"/>
-    <mergeCell ref="Y15:AA15"/>
-    <mergeCell ref="AB15:AD15"/>
-    <mergeCell ref="AE15:AG15"/>
-    <mergeCell ref="AH15:AJ15"/>
-    <mergeCell ref="AK15:AM15"/>
-    <mergeCell ref="AB14:AD14"/>
-    <mergeCell ref="AE14:AG14"/>
-    <mergeCell ref="AH14:AJ14"/>
-    <mergeCell ref="AH17:AJ17"/>
-    <mergeCell ref="AH18:AJ18"/>
-    <mergeCell ref="AK18:AM18"/>
-    <mergeCell ref="AE16:AG16"/>
-    <mergeCell ref="AH16:AJ16"/>
-    <mergeCell ref="AK16:AM16"/>
-    <mergeCell ref="AK17:AM17"/>
-    <mergeCell ref="AE18:AG18"/>
-    <mergeCell ref="AE17:AG17"/>
+    <mergeCell ref="V16:X16"/>
+    <mergeCell ref="Y16:AA16"/>
+    <mergeCell ref="P16:R16"/>
+    <mergeCell ref="Y14:AA14"/>
+    <mergeCell ref="AB16:AD16"/>
+    <mergeCell ref="S15:U15"/>
+    <mergeCell ref="V14:X14"/>
+    <mergeCell ref="AB17:AD17"/>
+    <mergeCell ref="AB18:AD18"/>
+    <mergeCell ref="J18:L18"/>
+    <mergeCell ref="M18:O18"/>
+    <mergeCell ref="P18:R18"/>
+    <mergeCell ref="S18:U18"/>
+    <mergeCell ref="V18:X18"/>
+    <mergeCell ref="Y18:AA18"/>
+    <mergeCell ref="V17:X17"/>
+    <mergeCell ref="Y17:AA17"/>
+    <mergeCell ref="S17:U17"/>
+    <mergeCell ref="P17:R17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2764,15 +2764,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010071E2E1765E21CD48A316A5744F1B35F1" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3716a12123983421c07d43acb73c349a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="34a395dc-6d6e-4dc0-a4c6-69ddff475736" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="74b1a612479c6867d4e6f74a081c53f8" ns2:_="">
     <xsd:import namespace="34a395dc-6d6e-4dc0-a4c6-69ddff475736"/>
@@ -2916,15 +2907,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E2A1BF69-AB93-44B6-9BDE-367FB52D1FA2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7F0FF976-C8BE-483D-8558-4A3260AB9DFF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2940,4 +2932,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E2A1BF69-AB93-44B6-9BDE-367FB52D1FA2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>